<commit_message>
changes at the table
</commit_message>
<xml_diff>
--- a/files/Tableau de synthèse.xlsx
+++ b/files/Tableau de synthèse.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -119,19 +119,31 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">GSB Frais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ü</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSB Visites</t>
+  </si>
+  <si>
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
     <t xml:space="preserve">Mise en ligne sur les réseaux sociaux du site créé</t>
   </si>
   <si>
-    <t xml:space="preserve">ü</t>
+    <t xml:space="preserve">Mise en place d’un trello et UML + user stories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place de WordPress non-installé sur le PC</t>
   </si>
   <si>
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t xml:space="preserve">J'ai amélioré le site internet interne du Médipôle de Savoie</t>
+    <t xml:space="preserve">J'ai amélioré le site internet interne du Médipôle de Savoie (trello, user stories)</t>
   </si>
   <si>
     <t xml:space="preserve">Mise en production et suivi utilisateur du projet final</t>
@@ -768,8 +780,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -915,22 +927,32 @@
       <c r="H8" s="17"/>
     </row>
     <row r="9" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
+      <c r="A9" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="H9" s="21"/>
     </row>
     <row r="10" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
+      <c r="A10" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="B10" s="22"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="G10" s="20"/>
       <c r="H10" s="21"/>
     </row>
@@ -1016,7 +1038,7 @@
     </row>
     <row r="19" s="16" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -1028,37 +1050,45 @@
     </row>
     <row r="20" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="21"/>
     </row>
     <row r="21" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18"/>
+      <c r="A21" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="B21" s="22"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="G21" s="20"/>
       <c r="H21" s="21"/>
     </row>
     <row r="22" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
+      <c r="A22" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="B22" s="22"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
+      <c r="H22" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
@@ -1102,7 +1132,7 @@
     </row>
     <row r="27" s="16" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -1114,21 +1144,21 @@
     </row>
     <row r="28" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
     </row>
     <row r="29" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B29" s="22"/>
       <c r="C29" s="20"/>
@@ -1136,18 +1166,18 @@
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H29" s="21"/>
     </row>
     <row r="30" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B30" s="22"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
@@ -1156,7 +1186,7 @@
     </row>
     <row r="31" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B31" s="22"/>
       <c r="C31" s="20"/>
@@ -1165,16 +1195,16 @@
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>

</xml_diff>

<commit_message>
modification page des stages
</commit_message>
<xml_diff>
--- a/files/Tableau de synthèse.xlsx
+++ b/files/Tableau de synthèse.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -34,13 +34,13 @@
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
   </si>
   <si>
-    <t xml:space="preserve">NOM et prénom : DEREPIERRE Alexandre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : 02146717364</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centre de formation : Lycée Gabriel Fauré</t>
+    <t xml:space="preserve">NOM et prénom : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° candidat : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre de formation :</t>
   </si>
   <si>
     <t xml:space="preserve">Option :</t>
@@ -49,10 +49,10 @@
     <t xml:space="preserve">▢ SISR</t>
   </si>
   <si>
-    <t xml:space="preserve"> SLAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresse URL du portfolio : https://crunchya.github.io</t>
+    <t xml:space="preserve">x SLAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse URL du portfolio :</t>
   </si>
   <si>
     <t xml:space="preserve">Compétences mises en œuvre
@@ -119,54 +119,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">GogMeteo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/10/21
-02/11/21</t>
+    <t xml:space="preserve">GSB Frais</t>
   </si>
   <si>
     <t xml:space="preserve">ü</t>
   </si>
   <si>
-    <t xml:space="preserve">GSB Android</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/12/221
-18/04/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSB Symfony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/12/21
-18/04/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veille Informatique</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">02/09/21
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="22"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">∞</t>
-    </r>
+    <t xml:space="preserve">GSB Visites</t>
   </si>
   <si>
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
@@ -175,14 +134,16 @@
     <t xml:space="preserve">Mise en ligne sur les réseaux sociaux du site créé</t>
   </si>
   <si>
+    <t xml:space="preserve">Mise en place d’un trello et UML + user stories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place de WordPress non-installé sur le PC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Réalisations en milieu professionnel en cours de seconde année</t>
   </si>
   <si>
-    <t xml:space="preserve">J'ai amélioré le site internet interne du Médipôle de Savoie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/01/22 
-18/02/22</t>
+    <t xml:space="preserve">J'ai amélioré le site internet interne du Médipôle de Savoie (trello, user stories)</t>
   </si>
   <si>
     <t xml:space="preserve">Mise en production et suivi utilisateur du projet final</t>
@@ -195,22 +156,17 @@
   </si>
   <si>
     <t xml:space="preserve">J’ai analysé, modifié et suivi les modifications apportées à la conformité par rapport au RGPD de l’application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/01/22
-18/02/22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -242,14 +198,6 @@
     <font>
       <b val="true"/>
       <sz val="18"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="18"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -290,17 +238,17 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="12"/>
       <name val="Wingdings"/>
       <family val="0"/>
       <charset val="2"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="22"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <sz val="12"/>
+      <name val="Wingdings"/>
+      <family val="0"/>
+      <charset val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -664,48 +612,48 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -716,20 +664,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -740,15 +688,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -825,48 +773,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>269640</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>377640</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12335400" y="1631880"/>
-          <a:ext cx="269640" cy="269640"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -874,8 +780,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1024,75 +930,51 @@
       <c r="A9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
       <c r="G9" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="21"/>
     </row>
     <row r="10" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B10" s="22"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>31</v>
-      </c>
+      <c r="A11" s="18"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>27</v>
-      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>33</v>
-      </c>
+      <c r="A12" s="18"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="21" t="s">
-        <v>27</v>
-      </c>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18"/>
@@ -1156,7 +1038,7 @@
     </row>
     <row r="19" s="16" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -1168,39 +1050,45 @@
     </row>
     <row r="20" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="19" t="n">
-        <v>44372</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B20" s="22"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="21"/>
     </row>
     <row r="21" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18"/>
+      <c r="A21" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="B21" s="22"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="20" t="s">
+        <v>26</v>
+      </c>
       <c r="G21" s="20"/>
       <c r="H21" s="21"/>
     </row>
     <row r="22" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
+      <c r="A22" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="B22" s="22"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
+      <c r="H22" s="21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
@@ -1244,7 +1132,7 @@
     </row>
     <row r="27" s="16" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -1256,46 +1144,40 @@
     </row>
     <row r="28" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>38</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B28" s="19"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
     </row>
     <row r="29" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="19" t="n">
-        <v>44607</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B29" s="22"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H29" s="21"/>
     </row>
     <row r="30" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>38</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B30" s="22"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
@@ -1304,29 +1186,25 @@
     </row>
     <row r="31" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="19" t="n">
-        <v>44563</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B31" s="22"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>43</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B32" s="22"/>
       <c r="C32" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
@@ -1379,9 +1257,6 @@
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="Adresse URL du portfolio : https://crunchya.github.io"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1389,6 +1264,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>